<commit_message>
xlxs for synthetoc++ic k=0.1
</commit_message>
<xml_diff>
--- a/results/real_data_freelancer_0.2_opt_constrained/results_freelancer_k=0.2.xlsx
+++ b/results/real_data_freelancer_0.2_opt_constrained/results_freelancer_k=0.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Konstantina\Desktop\HDrop20-Master-Thesis-Experiments\results\real_data_freelancer_0.2_opt_constrained\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7DCAE0-0D32-453C-8E91-580C91D3A001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4215D455-30EE-4704-9EE9-B068720936AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -155,7 +155,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,6 +249,15 @@
       <charset val="161"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="161"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -322,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -347,6 +356,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
@@ -630,7 +641,7 @@
   <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -719,7 +730,7 @@
       <c r="M2" s="7">
         <v>0.88432999999999995</v>
       </c>
-      <c r="N2" s="11">
+      <c r="N2" s="10">
         <f>AVERAGE(B2:M2)</f>
         <v>0.9312733333333334</v>
       </c>
@@ -826,7 +837,7 @@
       <c r="M5" s="7">
         <v>0.97309000000000001</v>
       </c>
-      <c r="N5" s="10">
+      <c r="N5" s="12">
         <f>AVERAGE(B5:M5)</f>
         <v>0.94791083333333326</v>
       </c>
@@ -1197,7 +1208,7 @@
       <c r="M18" s="7">
         <v>0.79825000000000002</v>
       </c>
-      <c r="N18" s="11">
+      <c r="N18" s="10">
         <f>AVERAGE(B18:M18)</f>
         <v>0.79216583333333324</v>
       </c>
@@ -1304,7 +1315,7 @@
       <c r="M21" s="7">
         <v>0.91803000000000001</v>
       </c>
-      <c r="N21" s="10">
+      <c r="N21" s="13">
         <f>AVERAGE(B21:M21)</f>
         <v>0.84353583333333348</v>
       </c>

</xml_diff>